<commit_message>
add a new file for example, add new data about date, day etc..
</commit_message>
<xml_diff>
--- a/python-toyProject/toyProject_timeManagement/Time.xlsx
+++ b/python-toyProject/toyProject_timeManagement/Time.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\toyProject_timeManagement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56509A13-1865-4858-A132-B0A853FD4660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD736E80-68B0-48B8-B9F1-104DFA382BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{36B8DAA8-34F7-40AA-8D19-6528CF3D8C6E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="140">
   <si>
     <t>기상시간:18시30분</t>
   </si>
@@ -676,6 +676,96 @@
       </rPr>
       <t>분</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">전공공부:4시간40분 </t>
+  </si>
+  <si>
+    <t>11월14(일</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>11</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>15(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="돋움"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>월</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11월16(화</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>11월20(토</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기상시간:11시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기상시간:10시30분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기상시간:9시10분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기상시간:10시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자기소개서_세메스:1시간17분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자기소개서_현대모비스:2시간01분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">자기소개서_KCC:1시간22분 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>면접_동원:1시간40분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자기소개서_오뚜기:50분</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자기소개서_LIG넥스원:2시간30분</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -683,7 +773,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -730,6 +820,13 @@
       <sz val="10"/>
       <color rgb="FF252525"/>
       <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="돋움"/>
       <family val="3"/>
       <charset val="129"/>
     </font>
@@ -1088,8 +1185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61DFE1BC-7273-4A37-817F-A50374F779FC}">
   <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.4"/>
@@ -1618,8 +1715,58 @@
         <v>120</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A47" s="3"/>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A43" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A44" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A46" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A114" s="3"/>

</xml_diff>